<commit_message>
added points, scene controller and spot controller
</commit_message>
<xml_diff>
--- a/Assets/points.xlsx
+++ b/Assets/points.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\unity\LIVR\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FFB55D43-951E-4A99-B6AA-CDA58C2C0726}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ADABD5C-C026-4BE1-AC21-7BDA94A3AE21}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17625" xr2:uid="{61B829DA-B794-4082-86F2-FF2620DF3C2B}"/>
   </bookViews>
@@ -490,7 +490,7 @@
   <dimension ref="A1:S26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="R24" sqref="R24"/>
+      <selection activeCell="AC14" sqref="AC14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>